<commit_message>
Admin: Alignment of code across all pages manipulated to make it a little more readable.
</commit_message>
<xml_diff>
--- a/functional-testing.xlsx
+++ b/functional-testing.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae6e5f45dd1637aa/Documents/Full Stack Course/MS1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul_\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{F65BE287-9F7B-41D4-B52E-F61F8FA73BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57E680EB-328D-4490-8D58-76C8EF406CD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B592BFE-4169-4A60-98BC-CA37BE523162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Initial Functional Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="After user testing &amp; feedback" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>Navbar</t>
   </si>
@@ -197,9 +198,6 @@
     <t>About Page</t>
   </si>
   <si>
-    <t>the get in touch hyperlink connect to the Get in Touch page</t>
-  </si>
-  <si>
     <t>Get in Touch Page</t>
   </si>
   <si>
@@ -237,6 +235,9 @@
   </si>
   <si>
     <t>Correctly filled out form returns correct information from Code Institute when submitted</t>
+  </si>
+  <si>
+    <t>the get in touch hyperlink connects to the Get in Touch page</t>
   </si>
 </sst>
 </file>
@@ -360,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,6 +382,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,14 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A87AE-CCFF-4881-BEAF-6D70C3416B6F}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,13 +737,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -783,7 +785,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="G4" s="14"/>
+      <c r="G4" s="10"/>
       <c r="H4" t="s">
         <v>47</v>
       </c>
@@ -888,15 +890,15 @@
       <c r="E15" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
@@ -910,13 +912,13 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -1017,13 +1019,13 @@
       <c r="G27" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
@@ -1064,7 +1066,7 @@
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="15"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1080,31 +1082,31 @@
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="15"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="12" t="s">
         <v>48</v>
       </c>
       <c r="B38" s="8"/>
@@ -1113,7 +1115,7 @@
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="8"/>
@@ -1122,7 +1124,7 @@
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="12" t="s">
         <v>50</v>
       </c>
       <c r="B40" s="8"/>
@@ -1131,7 +1133,7 @@
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B41" s="8"/>
@@ -1140,7 +1142,7 @@
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B42" s="8"/>
@@ -1149,40 +1151,40 @@
       <c r="E42" s="8"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="10"/>
+      <c r="B44" s="14"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="8"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="8"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -1190,7 +1192,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -1198,7 +1200,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -1206,7 +1208,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -1214,7 +1216,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -1222,31 +1224,31 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54" s="8"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="8"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56" s="8"/>
-      <c r="C56" s="17"/>
+      <c r="C56" s="13"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1263,4 +1265,551 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16873F5-DFA9-46F0-9E19-234F0CDAC837}">
+  <dimension ref="A1:H57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="74.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="13.21875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="G4" s="10"/>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="14"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="8"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
+      <c r="B48" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A47:D47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dev: Changed primary content div tag to 'Main' on all pages. Changed all divs containing the main page headings to the 'Header' tag. Fix: Media query CSS was nested and IE 11 was unable to respond to it, this was corrected. Regression testing run and functional-testing.xlsx updated with the results.
</commit_message>
<xml_diff>
--- a/functional-testing.xlsx
+++ b/functional-testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae6e5f45dd1637aa/Documents/Full Stack Course/MS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B592BFE-4169-4A60-98BC-CA37BE523162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{162E13D5-7C7D-420E-BBB5-82EC52B5DBD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Functional Testing" sheetId="1" r:id="rId1"/>
@@ -57,30 +57,15 @@
     <t>Menu item Releases links back to the Releases page</t>
   </si>
   <si>
-    <t>Menu item Artists links back to the Releases page</t>
-  </si>
-  <si>
-    <t>Menu item About links back to the Releases page</t>
-  </si>
-  <si>
-    <t>Menu item Get in Touch links back to the Releases page</t>
-  </si>
-  <si>
     <t>Footer</t>
   </si>
   <si>
-    <t>Sitewide components</t>
-  </si>
-  <si>
     <t>Text logo links back to the Releases page</t>
   </si>
   <si>
     <t>Image logo links back to the Releases page</t>
   </si>
   <si>
-    <t>Facbook link links to 8 Meg Stick Facebook page</t>
-  </si>
-  <si>
     <t>Twitter link links to 8 Meg Stick Twitter page</t>
   </si>
   <si>
@@ -238,6 +223,21 @@
   </si>
   <si>
     <t>the get in touch hyperlink connects to the Get in Touch page</t>
+  </si>
+  <si>
+    <t>Menu item Artists links back to the Artists page</t>
+  </si>
+  <si>
+    <t>Menu item About links back to the About page</t>
+  </si>
+  <si>
+    <t>Menu item Get in Touch links back to the Get in Touch page</t>
+  </si>
+  <si>
+    <t>Facebook link links to 8 Meg Stick Facebook page</t>
+  </si>
+  <si>
+    <t>Site-wide components</t>
   </si>
 </sst>
 </file>
@@ -390,6 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -402,7 +403,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A87AE-CCFF-4881-BEAF-6D70C3416B6F}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,13 +737,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="A1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -761,7 +761,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -774,12 +774,12 @@
       <c r="E3" s="7"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -787,7 +787,7 @@
       <c r="E4" s="8"/>
       <c r="G4" s="10"/>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -801,7 +801,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -810,7 +810,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -819,7 +819,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -828,7 +828,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -837,7 +837,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -846,7 +846,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -855,7 +855,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -864,7 +864,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -873,7 +873,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -882,7 +882,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -890,19 +890,19 @@
       <c r="E15" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="6"/>
@@ -912,38 +912,38 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -954,7 +954,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -965,7 +965,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -976,7 +976,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -987,7 +987,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -998,7 +998,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1019,32 +1019,32 @@
       <c r="G27" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="A29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="8"/>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="8"/>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1151,40 +1151,40 @@
       <c r="E42" s="8"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="14"/>
+      <c r="A44" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="15"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B45" s="8"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
+      <c r="A47" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="13"/>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="13"/>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="13"/>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16873F5-DFA9-46F0-9E19-234F0CDAC837}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,13 +1284,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="A1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1321,12 +1321,12 @@
       <c r="E3" s="7"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1334,7 +1334,7 @@
       <c r="E4" s="8"/>
       <c r="G4" s="10"/>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1437,19 +1437,19 @@
       <c r="E15" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="6"/>
@@ -1459,38 +1459,38 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1566,32 +1566,32 @@
       <c r="G27" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="A29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="8"/>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="8"/>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1672,7 +1672,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1698,40 +1698,40 @@
       <c r="E42" s="8"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="14"/>
+      <c r="A44" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="15"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B45" s="8"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
+      <c r="A47" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -1771,31 +1771,31 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B54" s="8"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B55" s="8"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B56" s="8"/>
-      <c r="C56" s="18"/>
+      <c r="C56" s="14"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -1803,12 +1803,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A47:D47"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A47:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>